<commit_message>
Increase data to 25k, clean data, and update all outputs
</commit_message>
<xml_diff>
--- a/feature_summary_statistics.xlsx
+++ b/feature_summary_statistics.xlsx
@@ -527,14 +527,18 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5.417574366242333</v>
+        <v>5.397147792810761</v>
       </c>
       <c r="D2" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F2" t="n">
-        <v>2.352107553040144</v>
+        <v>2.404201680285235</v>
       </c>
       <c r="G2" t="n">
         <v>4</v>
@@ -546,19 +550,19 @@
         <v>7</v>
       </c>
       <c r="J2" t="n">
-        <v>15</v>
+        <v>22.05911613983685</v>
       </c>
       <c r="K2" t="n">
         <v>2</v>
       </c>
       <c r="L2" t="n">
-        <v>9.593380122962499</v>
+        <v>9.898654904524985</v>
       </c>
       <c r="M2" t="n">
-        <v>0.4302613233961393</v>
+        <v>0.4756747257191328</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1917167509600581</v>
+        <v>0.325849490365369</v>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
@@ -577,14 +581,18 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5.396308570540651</v>
+        <v>5.51696</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F3" t="n">
-        <v>2.417451663031122</v>
+        <v>2.484149592590578</v>
       </c>
       <c r="G3" t="n">
         <v>4</v>
@@ -596,19 +604,19 @@
         <v>7</v>
       </c>
       <c r="J3" t="n">
-        <v>19.86665222580568</v>
+        <v>20</v>
       </c>
       <c r="K3" t="n">
         <v>2</v>
       </c>
       <c r="L3" t="n">
-        <v>9.697342923831179</v>
+        <v>10</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5146060509070594</v>
+        <v>0.5057776704877733</v>
       </c>
       <c r="N3" t="n">
-        <v>0.4949906974002545</v>
+        <v>0.3168348566186308</v>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
@@ -627,14 +635,18 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5.36140802462991</v>
+        <v>5.52352</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>2.419401653729865</v>
+        <v>2.507001837240746</v>
       </c>
       <c r="G4" t="n">
         <v>4</v>
@@ -646,19 +658,19 @@
         <v>7</v>
       </c>
       <c r="J4" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K4" t="n">
         <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>9.654850640035093</v>
+        <v>10</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4843545869216666</v>
+        <v>0.5074688792055595</v>
       </c>
       <c r="N4" t="n">
-        <v>0.4825317598459695</v>
+        <v>0.231383000082769</v>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
@@ -677,14 +689,18 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5.399373614517708</v>
+        <v>5.422834526525815</v>
       </c>
       <c r="D5" t="n">
         <v>5</v>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F5" t="n">
-        <v>2.412753304702142</v>
+        <v>2.408813531513111</v>
       </c>
       <c r="G5" t="n">
         <v>4</v>
@@ -696,19 +712,19 @@
         <v>7</v>
       </c>
       <c r="J5" t="n">
-        <v>15.3755771947849</v>
+        <v>17.14836723045121</v>
       </c>
       <c r="K5" t="n">
         <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>9.826796307889191</v>
+        <v>9.898974706645761</v>
       </c>
       <c r="M5" t="n">
-        <v>0.4703571373780482</v>
+        <v>0.4647157279304044</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1460196196495955</v>
+        <v>0.2726032057328682</v>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
@@ -727,14 +743,18 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5.406831252745763</v>
+        <v>5.419789535091943</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F6" t="n">
-        <v>2.429725792417945</v>
+        <v>2.432726768974609</v>
       </c>
       <c r="G6" t="n">
         <v>4</v>
@@ -746,19 +766,19 @@
         <v>7</v>
       </c>
       <c r="J6" t="n">
-        <v>17.7475861791701</v>
+        <v>20.38789569696585</v>
       </c>
       <c r="K6" t="n">
         <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>9.987155168464325</v>
+        <v>9.991532013808833</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4913726022548018</v>
+        <v>0.472047680146063</v>
       </c>
       <c r="N6" t="n">
-        <v>0.3032675829812757</v>
+        <v>0.2490580437577044</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
@@ -777,14 +797,18 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5.39543440184349</v>
+        <v>5.395155262871633</v>
       </c>
       <c r="D7" t="n">
         <v>5</v>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F7" t="n">
-        <v>2.431611244112174</v>
+        <v>2.422793641812492</v>
       </c>
       <c r="G7" t="n">
         <v>4</v>
@@ -796,19 +820,19 @@
         <v>7</v>
       </c>
       <c r="J7" t="n">
-        <v>16</v>
+        <v>18.32385999830354</v>
       </c>
       <c r="K7" t="n">
         <v>2</v>
       </c>
       <c r="L7" t="n">
-        <v>9.898900623506755</v>
+        <v>10</v>
       </c>
       <c r="M7" t="n">
-        <v>0.477525116572757</v>
+        <v>0.4733898976674009</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2044226869444765</v>
+        <v>0.1840545800350877</v>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
@@ -827,14 +851,18 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5.368370712027885</v>
+        <v>5.393953030575736</v>
       </c>
       <c r="D8" t="n">
         <v>5</v>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F8" t="n">
-        <v>2.405428360795885</v>
+        <v>2.419221381964977</v>
       </c>
       <c r="G8" t="n">
         <v>4</v>
@@ -846,19 +874,19 @@
         <v>7</v>
       </c>
       <c r="J8" t="n">
-        <v>17</v>
+        <v>17.33245276400199</v>
       </c>
       <c r="K8" t="n">
         <v>2</v>
       </c>
       <c r="L8" t="n">
-        <v>9.595262253443181</v>
+        <v>9.757651639634812</v>
       </c>
       <c r="M8" t="n">
-        <v>0.5016428314138476</v>
+        <v>0.5015354987072174</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3728107725940988</v>
+        <v>0.3116685297759028</v>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
@@ -877,14 +905,18 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5.447179643132253</v>
+        <v>5.49048</v>
       </c>
       <c r="D9" t="n">
         <v>5</v>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F9" t="n">
-        <v>2.41890218123675</v>
+        <v>2.495387434435365</v>
       </c>
       <c r="G9" t="n">
         <v>4</v>
@@ -896,19 +928,19 @@
         <v>7</v>
       </c>
       <c r="J9" t="n">
-        <v>16.92762575923046</v>
+        <v>17</v>
       </c>
       <c r="K9" t="n">
         <v>2</v>
       </c>
       <c r="L9" t="n">
-        <v>9.931096174848456</v>
+        <v>10</v>
       </c>
       <c r="M9" t="n">
-        <v>0.4895860833808575</v>
+        <v>0.483607971980951</v>
       </c>
       <c r="N9" t="n">
-        <v>0.299320927865693</v>
+        <v>0.2179145984647604</v>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
@@ -927,14 +959,18 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5.401527537562658</v>
+        <v>5.4978</v>
       </c>
       <c r="D10" t="n">
         <v>5</v>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F10" t="n">
-        <v>2.394633221768824</v>
+        <v>2.496862938365124</v>
       </c>
       <c r="G10" t="n">
         <v>4</v>
@@ -946,19 +982,19 @@
         <v>7</v>
       </c>
       <c r="J10" t="n">
-        <v>15.6385891811975</v>
+        <v>19</v>
       </c>
       <c r="K10" t="n">
         <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>9.888616388721939</v>
+        <v>10</v>
       </c>
       <c r="M10" t="n">
-        <v>0.4572648413211655</v>
+        <v>0.5086483897787066</v>
       </c>
       <c r="N10" t="n">
-        <v>0.2358981870839938</v>
+        <v>0.2920482016638655</v>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
@@ -977,14 +1013,18 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5.375035842268092</v>
+        <v>5.409618084266847</v>
       </c>
       <c r="D11" t="n">
         <v>5</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F11" t="n">
-        <v>2.41988065675526</v>
+        <v>2.4380173098928</v>
       </c>
       <c r="G11" t="n">
         <v>4</v>
@@ -996,19 +1036,19 @@
         <v>7</v>
       </c>
       <c r="J11" t="n">
-        <v>16.41598367440171</v>
+        <v>17.54312365613538</v>
       </c>
       <c r="K11" t="n">
         <v>2</v>
       </c>
       <c r="L11" t="n">
-        <v>9.922192006959426</v>
+        <v>9.988887373555405</v>
       </c>
       <c r="M11" t="n">
-        <v>0.535147424733975</v>
+        <v>0.4883438179841286</v>
       </c>
       <c r="N11" t="n">
-        <v>0.408935496271793</v>
+        <v>0.2538801138390108</v>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
@@ -1027,14 +1067,18 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5.390564429304008</v>
+        <v>5.388313356857467</v>
       </c>
       <c r="D12" t="n">
         <v>5</v>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F12" t="n">
-        <v>2.367748906119265</v>
+        <v>2.424553702145062</v>
       </c>
       <c r="G12" t="n">
         <v>4</v>
@@ -1046,19 +1090,19 @@
         <v>7</v>
       </c>
       <c r="J12" t="n">
-        <v>15.92245426240386</v>
+        <v>16.94862224620156</v>
       </c>
       <c r="K12" t="n">
         <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>9.801062296076122</v>
+        <v>9.915523175839434</v>
       </c>
       <c r="M12" t="n">
-        <v>0.4419047319617624</v>
+        <v>0.4452983794459147</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1905512405198029</v>
+        <v>0.1447175403472909</v>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
@@ -1077,14 +1121,18 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5.39866220284601</v>
+        <v>5.399606895218894</v>
       </c>
       <c r="D13" t="n">
         <v>5</v>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F13" t="n">
-        <v>2.419502686546994</v>
+        <v>2.416831141641192</v>
       </c>
       <c r="G13" t="n">
         <v>4</v>
@@ -1096,19 +1144,19 @@
         <v>7</v>
       </c>
       <c r="J13" t="n">
-        <v>16.18862209076082</v>
+        <v>18</v>
       </c>
       <c r="K13" t="n">
         <v>2</v>
       </c>
       <c r="L13" t="n">
-        <v>10</v>
+        <v>9.817613144443644</v>
       </c>
       <c r="M13" t="n">
-        <v>0.4821513944422301</v>
+        <v>0.4778272024974211</v>
       </c>
       <c r="N13" t="n">
-        <v>0.2314055049816028</v>
+        <v>0.1808095404691339</v>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
@@ -1127,38 +1175,42 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.696442777270927</v>
+        <v>2.65591051555896</v>
       </c>
       <c r="D14" t="n">
-        <v>2.510983961734181</v>
-      </c>
-      <c r="E14" t="inlineStr"/>
+        <v>2.479357374307295</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F14" t="n">
-        <v>1.6609492772331</v>
+        <v>1.667884188661627</v>
       </c>
       <c r="G14" t="n">
-        <v>1.451810172898504</v>
+        <v>1.381801228885102</v>
       </c>
       <c r="H14" t="n">
-        <v>2.510983961734181</v>
+        <v>2.479357374307295</v>
       </c>
       <c r="I14" t="n">
-        <v>3.786080630460188</v>
+        <v>3.809153797113572</v>
       </c>
       <c r="J14" t="n">
-        <v>8.724033514806848</v>
+        <v>9.214165475731303</v>
       </c>
       <c r="K14" t="n">
-        <v>0.3526342007755175</v>
+        <v>0.2523622111083583</v>
       </c>
       <c r="L14" t="n">
-        <v>5.673215669805288</v>
+        <v>5.708588046006935</v>
       </c>
       <c r="M14" t="n">
-        <v>0.4938861315521992</v>
+        <v>0.4574632988661474</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.01510190201609474</v>
+        <v>-0.1034906373862028</v>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
@@ -1177,38 +1229,42 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2.680148875600727</v>
+        <v>3.16412</v>
       </c>
       <c r="D15" t="n">
-        <v>2.487750973377035</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F15" t="n">
-        <v>1.679937029995052</v>
+        <v>1.680029025195999</v>
       </c>
       <c r="G15" t="n">
-        <v>1.429564841051964</v>
+        <v>2</v>
       </c>
       <c r="H15" t="n">
-        <v>2.487750973377035</v>
+        <v>3</v>
       </c>
       <c r="I15" t="n">
-        <v>3.760676711850627</v>
+        <v>4</v>
       </c>
       <c r="J15" t="n">
-        <v>8.43861956947428</v>
+        <v>10</v>
       </c>
       <c r="K15" t="n">
-        <v>0.3119660623544367</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>5.792540313363416</v>
+        <v>6</v>
       </c>
       <c r="M15" t="n">
-        <v>0.47217422002297</v>
+        <v>0.4653773431615975</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.1430287063286824</v>
+        <v>-0.06852633770822836</v>
       </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
@@ -1227,38 +1283,42 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.658664669518846</v>
+        <v>2.657822235389438</v>
       </c>
       <c r="D16" t="n">
-        <v>2.441755596506323</v>
-      </c>
-      <c r="E16" t="inlineStr"/>
+        <v>2.471489856024779</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F16" t="n">
-        <v>1.682624325887686</v>
+        <v>1.663290823260654</v>
       </c>
       <c r="G16" t="n">
-        <v>1.379148235608635</v>
+        <v>1.402706916924793</v>
       </c>
       <c r="H16" t="n">
-        <v>2.441755596506323</v>
+        <v>2.471489856024779</v>
       </c>
       <c r="I16" t="n">
-        <v>3.782768646119773</v>
+        <v>3.735384971605361</v>
       </c>
       <c r="J16" t="n">
-        <v>8.611331595310968</v>
+        <v>8.999371684843037</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2966402203990999</v>
+        <v>0.3185486674149971</v>
       </c>
       <c r="L16" t="n">
-        <v>5.756182327017241</v>
+        <v>5.691887403294705</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4881174167879303</v>
+        <v>0.491535732662787</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.1571904049444397</v>
+        <v>-0.08271533018914035</v>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
@@ -1277,38 +1337,42 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2.701965587062749</v>
+        <v>2.656939669089871</v>
       </c>
       <c r="D17" t="n">
-        <v>2.512786023759177</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
+        <v>2.455772405699695</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F17" t="n">
-        <v>1.685246204506996</v>
+        <v>1.663512999432618</v>
       </c>
       <c r="G17" t="n">
-        <v>1.411126172024903</v>
+        <v>1.412500933947608</v>
       </c>
       <c r="H17" t="n">
-        <v>2.512786023759177</v>
+        <v>2.455772405699695</v>
       </c>
       <c r="I17" t="n">
-        <v>3.814833271645049</v>
+        <v>3.747309159038525</v>
       </c>
       <c r="J17" t="n">
-        <v>8.686108408858075</v>
+        <v>9.09640385787336</v>
       </c>
       <c r="K17" t="n">
-        <v>0.3133787805463738</v>
+        <v>0.3194212870113798</v>
       </c>
       <c r="L17" t="n">
-        <v>5.783574674693768</v>
+        <v>5.696664740989578</v>
       </c>
       <c r="M17" t="n">
-        <v>0.4624713516902269</v>
+        <v>0.4892666192946246</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.1829957888736331</v>
+        <v>-0.09665079962777146</v>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
@@ -1327,38 +1391,42 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2.642977953286891</v>
+        <v>2.668783010156976</v>
       </c>
       <c r="D18" t="n">
-        <v>2.451671284195268</v>
-      </c>
-      <c r="E18" t="inlineStr"/>
+        <v>2.474618992031357</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F18" t="n">
-        <v>1.640325194557133</v>
+        <v>1.669455825937445</v>
       </c>
       <c r="G18" t="n">
-        <v>1.419780731361177</v>
+        <v>1.407424373936286</v>
       </c>
       <c r="H18" t="n">
-        <v>2.451671284195268</v>
+        <v>2.474618992031357</v>
       </c>
       <c r="I18" t="n">
-        <v>3.671077462846953</v>
+        <v>3.762669796497288</v>
       </c>
       <c r="J18" t="n">
-        <v>8.741007421851736</v>
+        <v>9.494028870234665</v>
       </c>
       <c r="K18" t="n">
-        <v>0.3305013095249938</v>
+        <v>0.3277987065740914</v>
       </c>
       <c r="L18" t="n">
-        <v>5.68560861898329</v>
+        <v>5.704123129453413</v>
       </c>
       <c r="M18" t="n">
-        <v>0.5295274839203877</v>
+        <v>0.474422956614366</v>
       </c>
       <c r="N18" t="n">
-        <v>0.01048558068794314</v>
+        <v>-0.08645127552233767</v>
       </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
@@ -1377,38 +1445,42 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2.6167186456094</v>
+        <v>3.16632</v>
       </c>
       <c r="D19" t="n">
-        <v>2.39941806296528</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F19" t="n">
-        <v>1.641360322360854</v>
+        <v>1.689962099124078</v>
       </c>
       <c r="G19" t="n">
-        <v>1.381677989753688</v>
+        <v>2</v>
       </c>
       <c r="H19" t="n">
-        <v>2.39941806296528</v>
+        <v>3</v>
       </c>
       <c r="I19" t="n">
-        <v>3.719817192234386</v>
+        <v>4</v>
       </c>
       <c r="J19" t="n">
-        <v>9.069898539068269</v>
+        <v>9</v>
       </c>
       <c r="K19" t="n">
-        <v>0.3400475091613168</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
-        <v>5.578341578018263</v>
+        <v>6</v>
       </c>
       <c r="M19" t="n">
-        <v>0.4991662054611931</v>
+        <v>0.4693636736386789</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.07903519202546638</v>
+        <v>-0.09039216520414906</v>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="n">
@@ -1427,38 +1499,42 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2.640689960810297</v>
+        <v>2.661967829570862</v>
       </c>
       <c r="D20" t="n">
-        <v>2.456390198632318</v>
-      </c>
-      <c r="E20" t="inlineStr"/>
+        <v>2.474871387275789</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F20" t="n">
-        <v>1.636658742656488</v>
+        <v>1.665817979309238</v>
       </c>
       <c r="G20" t="n">
-        <v>1.41277262519214</v>
+        <v>1.406145357527424</v>
       </c>
       <c r="H20" t="n">
-        <v>2.456390198632318</v>
+        <v>2.474871387275789</v>
       </c>
       <c r="I20" t="n">
-        <v>3.68913128847205</v>
+        <v>3.736466608155481</v>
       </c>
       <c r="J20" t="n">
-        <v>8.63369501802185</v>
+        <v>8.975201817859316</v>
       </c>
       <c r="K20" t="n">
-        <v>0.3351640941361934</v>
+        <v>0.3247735003499505</v>
       </c>
       <c r="L20" t="n">
-        <v>5.602588344016133</v>
+        <v>5.677425097109813</v>
       </c>
       <c r="M20" t="n">
-        <v>0.4787435741101637</v>
+        <v>0.4663349296663823</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.06687137393589682</v>
+        <v>-0.1014824425665335</v>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="n">
@@ -1477,38 +1553,42 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.617227001006745</v>
+        <v>2.653834642961382</v>
       </c>
       <c r="D21" t="n">
-        <v>2.402588765071173</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
+        <v>2.460019756208289</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F21" t="n">
-        <v>1.655571336293794</v>
+        <v>1.663408785290187</v>
       </c>
       <c r="G21" t="n">
-        <v>1.384526229260436</v>
+        <v>1.40850198416736</v>
       </c>
       <c r="H21" t="n">
-        <v>2.402588765071173</v>
+        <v>2.460019756208289</v>
       </c>
       <c r="I21" t="n">
-        <v>3.65086664426502</v>
+        <v>3.719551379806643</v>
       </c>
       <c r="J21" t="n">
-        <v>8.997170507240739</v>
+        <v>9.36415747094745</v>
       </c>
       <c r="K21" t="n">
-        <v>0.3274573819473971</v>
+        <v>0.3220034653839376</v>
       </c>
       <c r="L21" t="n">
-        <v>5.669870885473921</v>
+        <v>5.684745954847663</v>
       </c>
       <c r="M21" t="n">
-        <v>0.5410853077122864</v>
+        <v>0.4852339032266641</v>
       </c>
       <c r="N21" t="n">
-        <v>0.03715970427358828</v>
+        <v>-0.06660203956364841</v>
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
@@ -1527,38 +1607,42 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.635174096750581</v>
+        <v>2.668522437679055</v>
       </c>
       <c r="D22" t="n">
-        <v>2.428424310413755</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
+        <v>2.478076348765539</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F22" t="n">
-        <v>1.670543560266805</v>
+        <v>1.654341496417919</v>
       </c>
       <c r="G22" t="n">
-        <v>1.421841342249167</v>
+        <v>1.42968373306543</v>
       </c>
       <c r="H22" t="n">
-        <v>2.428424310413755</v>
+        <v>2.478076348765539</v>
       </c>
       <c r="I22" t="n">
-        <v>3.710333709755657</v>
+        <v>3.745876968508127</v>
       </c>
       <c r="J22" t="n">
-        <v>8.781716787378018</v>
+        <v>8.881663131511267</v>
       </c>
       <c r="K22" t="n">
-        <v>0.2803074662136638</v>
+        <v>0.3250424377298148</v>
       </c>
       <c r="L22" t="n">
-        <v>5.681098653164001</v>
+        <v>5.671752786072967</v>
       </c>
       <c r="M22" t="n">
-        <v>0.4900463876004443</v>
+        <v>0.4591088962503334</v>
       </c>
       <c r="N22" t="n">
-        <v>-0.003281646526659632</v>
+        <v>-0.1077686068196884</v>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
@@ -1577,38 +1661,42 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.681082595841988</v>
+        <v>2.647688601369092</v>
       </c>
       <c r="D23" t="n">
-        <v>2.525015895413125</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
+        <v>2.451906016235691</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F23" t="n">
-        <v>1.660072145981542</v>
+        <v>1.668331993363924</v>
       </c>
       <c r="G23" t="n">
-        <v>1.443770259574922</v>
+        <v>1.388306154653602</v>
       </c>
       <c r="H23" t="n">
-        <v>2.525015895413125</v>
+        <v>2.451906016235691</v>
       </c>
       <c r="I23" t="n">
-        <v>3.775007289214044</v>
+        <v>3.729761900678151</v>
       </c>
       <c r="J23" t="n">
-        <v>8.568802984780115</v>
+        <v>8.966096519446197</v>
       </c>
       <c r="K23" t="n">
-        <v>0.2699566902434949</v>
+        <v>0.3169247852661575</v>
       </c>
       <c r="L23" t="n">
-        <v>5.667350343016081</v>
+        <v>5.698332229556094</v>
       </c>
       <c r="M23" t="n">
-        <v>0.3876359821562569</v>
+        <v>0.4936894671407192</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.1794104302999089</v>
+        <v>-0.07712962989762406</v>
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
@@ -1627,38 +1715,42 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2.682171008978177</v>
+        <v>2.650640043858628</v>
       </c>
       <c r="D24" t="n">
-        <v>2.471573001690314</v>
-      </c>
-      <c r="E24" t="inlineStr"/>
+        <v>2.460891436855539</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F24" t="n">
-        <v>1.690292587629167</v>
+        <v>1.659097593745479</v>
       </c>
       <c r="G24" t="n">
-        <v>1.419055555848971</v>
+        <v>1.400000105770897</v>
       </c>
       <c r="H24" t="n">
-        <v>2.471573001690314</v>
+        <v>2.460891436855539</v>
       </c>
       <c r="I24" t="n">
-        <v>3.741802363241344</v>
+        <v>3.730044962941731</v>
       </c>
       <c r="J24" t="n">
-        <v>9.12607983374798</v>
+        <v>9.382622279194498</v>
       </c>
       <c r="K24" t="n">
-        <v>0.3290215719475034</v>
+        <v>0.3229855786603969</v>
       </c>
       <c r="L24" t="n">
-        <v>5.821351945794813</v>
+        <v>5.668805145155248</v>
       </c>
       <c r="M24" t="n">
-        <v>0.5482630694186799</v>
+        <v>0.4679609589478448</v>
       </c>
       <c r="N24" t="n">
-        <v>-0.01400784072798222</v>
+        <v>-0.127776720623523</v>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
@@ -1677,38 +1769,42 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2.662718616213886</v>
+        <v>2.649436094318072</v>
       </c>
       <c r="D25" t="n">
-        <v>2.492882860411338</v>
-      </c>
-      <c r="E25" t="inlineStr"/>
+        <v>2.440824138566845</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F25" t="n">
-        <v>1.642708120204889</v>
+        <v>1.67006405218397</v>
       </c>
       <c r="G25" t="n">
-        <v>1.421278846617467</v>
+        <v>1.389127546978294</v>
       </c>
       <c r="H25" t="n">
-        <v>2.492882860411338</v>
+        <v>2.440824138566845</v>
       </c>
       <c r="I25" t="n">
-        <v>3.750216318498739</v>
+        <v>3.718108769452857</v>
       </c>
       <c r="J25" t="n">
-        <v>8.291691580539194</v>
+        <v>9.48785685934797</v>
       </c>
       <c r="K25" t="n">
-        <v>0.3000509241188903</v>
+        <v>0.3324193171917588</v>
       </c>
       <c r="L25" t="n">
-        <v>5.554470718476318</v>
+        <v>5.744270768244998</v>
       </c>
       <c r="M25" t="n">
-        <v>0.4188747528009428</v>
+        <v>0.5230003696126532</v>
       </c>
       <c r="N25" t="n">
-        <v>-0.1924087409997917</v>
+        <v>-0.04919441373970557</v>
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
@@ -1727,38 +1823,42 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>30.00884286707799</v>
+        <v>30.46692</v>
       </c>
       <c r="D26" t="n">
-        <v>29.93463345521945</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
+        <v>31</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F26" t="n">
-        <v>12.09080424832093</v>
+        <v>12.02947272502672</v>
       </c>
       <c r="G26" t="n">
-        <v>21.91167853950584</v>
+        <v>22</v>
       </c>
       <c r="H26" t="n">
-        <v>29.93463345521945</v>
+        <v>31</v>
       </c>
       <c r="I26" t="n">
-        <v>38.40128727012937</v>
+        <v>39</v>
       </c>
       <c r="J26" t="n">
-        <v>74.72905012436429</v>
+        <v>79</v>
       </c>
       <c r="K26" t="n">
-        <v>10.2402073664186</v>
+        <v>11</v>
       </c>
       <c r="L26" t="n">
-        <v>49.96360677897204</v>
+        <v>50</v>
       </c>
       <c r="M26" t="n">
-        <v>-0.02924317727078436</v>
+        <v>-0.003908085847358992</v>
       </c>
       <c r="N26" t="n">
-        <v>-0.003527482738006071</v>
+        <v>-0.03914101656307212</v>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
@@ -1777,38 +1877,42 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>30.3494901683966</v>
+        <v>29.98656763467655</v>
       </c>
       <c r="D27" t="n">
-        <v>30.38098597383651</v>
-      </c>
-      <c r="E27" t="inlineStr"/>
+        <v>29.92554109858022</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F27" t="n">
-        <v>12.09478031572074</v>
+        <v>11.97351453156817</v>
       </c>
       <c r="G27" t="n">
-        <v>22.12601786031331</v>
+        <v>22.00087270757546</v>
       </c>
       <c r="H27" t="n">
-        <v>30.38098597383651</v>
+        <v>29.92554109858022</v>
       </c>
       <c r="I27" t="n">
-        <v>38.50737144616182</v>
+        <v>38.12427663618003</v>
       </c>
       <c r="J27" t="n">
-        <v>74.89869317764004</v>
+        <v>75.29749270337092</v>
       </c>
       <c r="K27" t="n">
-        <v>10.47418220778919</v>
+        <v>10.37046770014287</v>
       </c>
       <c r="L27" t="n">
-        <v>50.24393072492069</v>
+        <v>49.73966923712142</v>
       </c>
       <c r="M27" t="n">
-        <v>0.02599841888868794</v>
+        <v>-0.01424687890734277</v>
       </c>
       <c r="N27" t="n">
-        <v>0.05349899284060378</v>
+        <v>-0.0003708654939482692</v>
       </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="n">
@@ -1829,7 +1933,7 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -1859,38 +1963,42 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>29.93197266775944</v>
+        <v>29.98546159886723</v>
       </c>
       <c r="D29" t="n">
-        <v>29.97217705139434</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
+        <v>29.92505657308295</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F29" t="n">
-        <v>12.15423718597047</v>
+        <v>11.95175010929368</v>
       </c>
       <c r="G29" t="n">
-        <v>21.83448606458025</v>
+        <v>21.91182924506917</v>
       </c>
       <c r="H29" t="n">
-        <v>29.97217705139434</v>
+        <v>29.92505657308295</v>
       </c>
       <c r="I29" t="n">
-        <v>38.08588097045664</v>
+        <v>37.9840821679361</v>
       </c>
       <c r="J29" t="n">
-        <v>84.32140671912327</v>
+        <v>85.31044155476656</v>
       </c>
       <c r="K29" t="n">
-        <v>9.492222360254424</v>
+        <v>10.34612882394376</v>
       </c>
       <c r="L29" t="n">
-        <v>49.84210951410488</v>
+        <v>49.64783133963594</v>
       </c>
       <c r="M29" t="n">
-        <v>-0.008751201261535611</v>
+        <v>-0.009080503942937234</v>
       </c>
       <c r="N29" t="n">
-        <v>0.07446338001140562</v>
+        <v>-0.007393634806731608</v>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="n">
@@ -1909,38 +2017,42 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>29.82151534260977</v>
+        <v>30.00915872242861</v>
       </c>
       <c r="D30" t="n">
-        <v>30.13796814973851</v>
-      </c>
-      <c r="E30" t="inlineStr"/>
+        <v>29.99135859791237</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F30" t="n">
-        <v>11.89408561771215</v>
+        <v>12.04844662184948</v>
       </c>
       <c r="G30" t="n">
-        <v>21.70155575915199</v>
+        <v>21.76040062559216</v>
       </c>
       <c r="H30" t="n">
-        <v>30.13796814973851</v>
+        <v>29.99135859791237</v>
       </c>
       <c r="I30" t="n">
-        <v>37.65413974896024</v>
+        <v>38.21638430043809</v>
       </c>
       <c r="J30" t="n">
-        <v>71.31170972808096</v>
+        <v>84.98014367980917</v>
       </c>
       <c r="K30" t="n">
-        <v>10.22504942945312</v>
+        <v>10.31286244657859</v>
       </c>
       <c r="L30" t="n">
-        <v>49.10643121648438</v>
+        <v>49.95570516091401</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.01053120251879457</v>
+        <v>0.01661038374976305</v>
       </c>
       <c r="N30" t="n">
-        <v>-7.32427768612709e-05</v>
+        <v>-0.02837169231003012</v>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="n">
@@ -1961,7 +2073,7 @@
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
@@ -1991,38 +2103,42 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>30.21582271800148</v>
+        <v>30.05829473809221</v>
       </c>
       <c r="D32" t="n">
-        <v>30.36264291962919</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
+        <v>30.0350933072145</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F32" t="n">
-        <v>11.94887927965833</v>
+        <v>11.94951119137398</v>
       </c>
       <c r="G32" t="n">
-        <v>22.35585547326098</v>
+        <v>22.00358836504404</v>
       </c>
       <c r="H32" t="n">
-        <v>30.36264291962919</v>
+        <v>30.0350933072145</v>
       </c>
       <c r="I32" t="n">
-        <v>38.36132121092025</v>
+        <v>38.06129568315909</v>
       </c>
       <c r="J32" t="n">
-        <v>69.52287830216609</v>
+        <v>80.14581225625783</v>
       </c>
       <c r="K32" t="n">
-        <v>10.16815046376204</v>
+        <v>10.51414822607414</v>
       </c>
       <c r="L32" t="n">
-        <v>49.74427701062005</v>
+        <v>49.76250828235823</v>
       </c>
       <c r="M32" t="n">
-        <v>-0.0544107693648305</v>
+        <v>0.003969665683025266</v>
       </c>
       <c r="N32" t="n">
-        <v>-0.02483768697617217</v>
+        <v>0.09381901291202643</v>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="n">
@@ -2041,38 +2157,42 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>30.05070739996551</v>
+        <v>30.01889417510183</v>
       </c>
       <c r="D33" t="n">
-        <v>30.18990206536628</v>
-      </c>
-      <c r="E33" t="inlineStr"/>
+        <v>29.97882122236578</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F33" t="n">
-        <v>12.18847912583554</v>
+        <v>12.03209435492214</v>
       </c>
       <c r="G33" t="n">
-        <v>22.07641049169115</v>
+        <v>21.96070893713815</v>
       </c>
       <c r="H33" t="n">
-        <v>30.18990206536628</v>
+        <v>29.97882122236578</v>
       </c>
       <c r="I33" t="n">
-        <v>38.31325352976231</v>
+        <v>38.15245204759672</v>
       </c>
       <c r="J33" t="n">
-        <v>76.63253015600201</v>
+        <v>81.92827491761527</v>
       </c>
       <c r="K33" t="n">
-        <v>9.639087459664058</v>
+        <v>10.27634974087522</v>
       </c>
       <c r="L33" t="n">
-        <v>50.12345198384021</v>
+        <v>49.84142440729012</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.04009878272542587</v>
+        <v>0.007424633820511482</v>
       </c>
       <c r="N33" t="n">
-        <v>0.03469139709290925</v>
+        <v>0.04258692752221016</v>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="n">
@@ -2123,38 +2243,42 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>30.04908619171239</v>
+        <v>30.6416</v>
       </c>
       <c r="D35" t="n">
-        <v>29.89858224438649</v>
-      </c>
-      <c r="E35" t="inlineStr"/>
+        <v>31</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F35" t="n">
-        <v>12.12227071839421</v>
+        <v>12.15221529160259</v>
       </c>
       <c r="G35" t="n">
-        <v>21.81149881499534</v>
+        <v>22</v>
       </c>
       <c r="H35" t="n">
-        <v>29.89858224438649</v>
+        <v>31</v>
       </c>
       <c r="I35" t="n">
-        <v>38.30363248513049</v>
+        <v>39</v>
       </c>
       <c r="J35" t="n">
-        <v>72.53294708380734</v>
+        <v>81</v>
       </c>
       <c r="K35" t="n">
-        <v>10.19743379060892</v>
+        <v>11</v>
       </c>
       <c r="L35" t="n">
-        <v>49.8996709217276</v>
+        <v>51</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.007276270781814046</v>
+        <v>0.01956726529554709</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.08631542256320524</v>
+        <v>-0.04518165609659075</v>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="n">
@@ -2173,38 +2297,42 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>30.09437240119672</v>
+        <v>30.4516</v>
       </c>
       <c r="D36" t="n">
-        <v>30.13127009416566</v>
-      </c>
-      <c r="E36" t="inlineStr"/>
+        <v>30</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F36" t="n">
-        <v>11.861818452678</v>
+        <v>11.97652516075498</v>
       </c>
       <c r="G36" t="n">
-        <v>21.92250113446066</v>
+        <v>22</v>
       </c>
       <c r="H36" t="n">
-        <v>30.13127009416566</v>
+        <v>30</v>
       </c>
       <c r="I36" t="n">
-        <v>38.20693280504314</v>
+        <v>38</v>
       </c>
       <c r="J36" t="n">
-        <v>81.739036446764</v>
+        <v>82</v>
       </c>
       <c r="K36" t="n">
-        <v>10.88315927306712</v>
+        <v>11</v>
       </c>
       <c r="L36" t="n">
-        <v>49.37891253115845</v>
+        <v>50</v>
       </c>
       <c r="M36" t="n">
-        <v>0.02337592771142595</v>
+        <v>0.01500972236590155</v>
       </c>
       <c r="N36" t="n">
-        <v>-0.07196663553670524</v>
+        <v>-0.001425019644812231</v>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="n">
@@ -2223,38 +2351,42 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>9.55674249568901</v>
+        <v>9.326362613100553</v>
       </c>
       <c r="D37" t="n">
-        <v>6.426922644764512</v>
-      </c>
-      <c r="E37" t="inlineStr"/>
+        <v>6.301590837744993</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F37" t="n">
-        <v>10.41996510659644</v>
+        <v>10.02294493170867</v>
       </c>
       <c r="G37" t="n">
-        <v>2.360910239587359</v>
+        <v>2.304749607342863</v>
       </c>
       <c r="H37" t="n">
-        <v>6.426922644764512</v>
+        <v>6.301590837744993</v>
       </c>
       <c r="I37" t="n">
-        <v>13.69738930917485</v>
+        <v>13.28170891612494</v>
       </c>
       <c r="J37" t="n">
-        <v>100.7330630365801</v>
+        <v>108.7239884683104</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.2514140951143579</v>
+        <v>0.002184496099511045</v>
       </c>
       <c r="L37" t="n">
-        <v>30.24311024197032</v>
+        <v>29.31155219838792</v>
       </c>
       <c r="M37" t="n">
-        <v>2.020301566509819</v>
+        <v>1.947271452661993</v>
       </c>
       <c r="N37" t="n">
-        <v>6.355966148749749</v>
+        <v>5.689386103580066</v>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="n">
@@ -2273,38 +2405,42 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>9.317955614120248</v>
+        <v>9.46145295806949</v>
       </c>
       <c r="D38" t="n">
-        <v>6.250078331507805</v>
-      </c>
-      <c r="E38" t="inlineStr"/>
+        <v>6.456445886025874</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F38" t="n">
-        <v>10.2887823332669</v>
+        <v>10.10007094357692</v>
       </c>
       <c r="G38" t="n">
-        <v>2.195709727853322</v>
+        <v>2.374920517819284</v>
       </c>
       <c r="H38" t="n">
-        <v>6.250078331507805</v>
+        <v>6.456445886025874</v>
       </c>
       <c r="I38" t="n">
-        <v>13.13763937450009</v>
+        <v>13.44487622188651</v>
       </c>
       <c r="J38" t="n">
-        <v>94.51353394554178</v>
+        <v>90.85134243622065</v>
       </c>
       <c r="K38" t="n">
-        <v>-0.1815334242442556</v>
+        <v>-0.04129384419471333</v>
       </c>
       <c r="L38" t="n">
-        <v>29.47229366314167</v>
+        <v>29.72251763707968</v>
       </c>
       <c r="M38" t="n">
-        <v>2.092525467414193</v>
+        <v>1.880865544897827</v>
       </c>
       <c r="N38" t="n">
-        <v>6.621777495375024</v>
+        <v>5.085299924548051</v>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="n">
@@ -2323,38 +2459,42 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>9.24651597934573</v>
+        <v>9.35518104256874</v>
       </c>
       <c r="D39" t="n">
-        <v>6.295050774000313</v>
-      </c>
-      <c r="E39" t="inlineStr"/>
+        <v>6.402610734373244</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F39" t="n">
-        <v>9.895598232321234</v>
+        <v>10.00587701599392</v>
       </c>
       <c r="G39" t="n">
-        <v>2.271757142877466</v>
+        <v>2.374660822105541</v>
       </c>
       <c r="H39" t="n">
-        <v>6.295050774000313</v>
+        <v>6.402610734373244</v>
       </c>
       <c r="I39" t="n">
-        <v>13.18589711445887</v>
+        <v>13.18102259730402</v>
       </c>
       <c r="J39" t="n">
-        <v>89.65953599237558</v>
+        <v>109.2334045022959</v>
       </c>
       <c r="K39" t="n">
-        <v>-0.1505906213363058</v>
+        <v>-0.1035692137934033</v>
       </c>
       <c r="L39" t="n">
-        <v>29.30262811067283</v>
+        <v>29.0930298055911</v>
       </c>
       <c r="M39" t="n">
-        <v>1.881518675389026</v>
+        <v>1.957408682079766</v>
       </c>
       <c r="N39" t="n">
-        <v>5.159029101536273</v>
+        <v>5.880428269273994</v>
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="n">
@@ -2373,38 +2513,42 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>9.560578072110005</v>
+        <v>9.888920000000001</v>
       </c>
       <c r="D40" t="n">
-        <v>6.488257867609813</v>
-      </c>
-      <c r="E40" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F40" t="n">
-        <v>10.11669526416736</v>
+        <v>10.0653859197424</v>
       </c>
       <c r="G40" t="n">
-        <v>2.27827127944263</v>
+        <v>3</v>
       </c>
       <c r="H40" t="n">
-        <v>6.488257867609813</v>
+        <v>7</v>
       </c>
       <c r="I40" t="n">
-        <v>13.87777944261603</v>
+        <v>14</v>
       </c>
       <c r="J40" t="n">
-        <v>79.03675587007935</v>
+        <v>117</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.02555309730080553</v>
+        <v>0</v>
       </c>
       <c r="L40" t="n">
-        <v>29.9346286855669</v>
+        <v>30</v>
       </c>
       <c r="M40" t="n">
-        <v>1.745700424385864</v>
+        <v>1.95728073584578</v>
       </c>
       <c r="N40" t="n">
-        <v>4.161630567460488</v>
+        <v>5.953175111705223</v>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="n">
@@ -2423,38 +2567,42 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>9.47925319281148</v>
+        <v>9.89664</v>
       </c>
       <c r="D41" t="n">
-        <v>6.589220445429364</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
+        <v>7</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F41" t="n">
-        <v>9.940579106844382</v>
+        <v>10.04942567257721</v>
       </c>
       <c r="G41" t="n">
-        <v>2.46314317490037</v>
+        <v>3</v>
       </c>
       <c r="H41" t="n">
-        <v>6.589220445429364</v>
+        <v>7</v>
       </c>
       <c r="I41" t="n">
-        <v>13.56662784583813</v>
+        <v>14</v>
       </c>
       <c r="J41" t="n">
-        <v>76.02511244848054</v>
+        <v>101</v>
       </c>
       <c r="K41" t="n">
-        <v>-0.06248580537602931</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>29.80461659691888</v>
+        <v>30</v>
       </c>
       <c r="M41" t="n">
-        <v>1.771706531948384</v>
+        <v>1.96167205046584</v>
       </c>
       <c r="N41" t="n">
-        <v>4.282878814912805</v>
+        <v>5.796018755703692</v>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="n">
@@ -2473,38 +2621,42 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>8.85513705697163</v>
+        <v>9.407270732560736</v>
       </c>
       <c r="D42" t="n">
-        <v>6.106009805547876</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
+        <v>6.359661495141305</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F42" t="n">
-        <v>9.377588751781696</v>
+        <v>10.11606444223571</v>
       </c>
       <c r="G42" t="n">
-        <v>2.145364255448009</v>
+        <v>2.338328178833868</v>
       </c>
       <c r="H42" t="n">
-        <v>6.106009805547876</v>
+        <v>6.359661495141305</v>
       </c>
       <c r="I42" t="n">
-        <v>12.73916247909691</v>
+        <v>13.43447617471599</v>
       </c>
       <c r="J42" t="n">
-        <v>70.69779233681433</v>
+        <v>108.218405327988</v>
       </c>
       <c r="K42" t="n">
-        <v>-0.2200406016851406</v>
+        <v>-0.09342543783843904</v>
       </c>
       <c r="L42" t="n">
-        <v>27.83439374896936</v>
+        <v>29.31957589742491</v>
       </c>
       <c r="M42" t="n">
-        <v>1.796143611187308</v>
+        <v>1.954152249626463</v>
       </c>
       <c r="N42" t="n">
-        <v>4.598864372527395</v>
+        <v>5.912113787786083</v>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="n">
@@ -2523,38 +2675,42 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>9.56581627022277</v>
+        <v>9.522451260271565</v>
       </c>
       <c r="D43" t="n">
-        <v>6.48522134363664</v>
-      </c>
-      <c r="E43" t="inlineStr"/>
+        <v>6.438866490765682</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F43" t="n">
-        <v>10.38710248122447</v>
+        <v>10.24552527588412</v>
       </c>
       <c r="G43" t="n">
-        <v>2.331257470525466</v>
+        <v>2.357357846737711</v>
       </c>
       <c r="H43" t="n">
-        <v>6.48522134363664</v>
+        <v>6.438866490765682</v>
       </c>
       <c r="I43" t="n">
-        <v>13.42442047969735</v>
+        <v>13.53120728327793</v>
       </c>
       <c r="J43" t="n">
-        <v>88.45593282645345</v>
+        <v>111.4602463971021</v>
       </c>
       <c r="K43" t="n">
-        <v>-0.240446769206484</v>
+        <v>-0.1316268544231226</v>
       </c>
       <c r="L43" t="n">
-        <v>30.7772806660767</v>
+        <v>29.96813514850484</v>
       </c>
       <c r="M43" t="n">
-        <v>1.918004864439959</v>
+        <v>1.973038094463437</v>
       </c>
       <c r="N43" t="n">
-        <v>5.27923965449884</v>
+        <v>6.156210654578517</v>
       </c>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="n">
@@ -2573,38 +2729,42 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>9.39495321946557</v>
+        <v>9.401734000840163</v>
       </c>
       <c r="D44" t="n">
-        <v>6.115563510886723</v>
-      </c>
-      <c r="E44" t="inlineStr"/>
+        <v>6.479174027485016</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F44" t="n">
-        <v>10.20129989225525</v>
+        <v>10.02028988541035</v>
       </c>
       <c r="G44" t="n">
-        <v>2.415142410954346</v>
+        <v>2.330091598595597</v>
       </c>
       <c r="H44" t="n">
-        <v>6.115563510886723</v>
+        <v>6.479174027485016</v>
       </c>
       <c r="I44" t="n">
-        <v>13.41623116671386</v>
+        <v>13.42695316292541</v>
       </c>
       <c r="J44" t="n">
-        <v>89.52246267580412</v>
+        <v>97.07330963146549</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.09769356552118252</v>
+        <v>-0.07797418160878719</v>
       </c>
       <c r="L44" t="n">
-        <v>29.04061797330741</v>
+        <v>29.09322499972554</v>
       </c>
       <c r="M44" t="n">
-        <v>1.968435848318796</v>
+        <v>1.906146591025035</v>
       </c>
       <c r="N44" t="n">
-        <v>5.729406603563518</v>
+        <v>5.449426322137141</v>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="n">
@@ -2623,38 +2783,42 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>9.265284998328763</v>
+        <v>9.459154219354259</v>
       </c>
       <c r="D45" t="n">
-        <v>6.375478470430767</v>
-      </c>
-      <c r="E45" t="inlineStr"/>
+        <v>6.403334235929634</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F45" t="n">
-        <v>9.924197630598924</v>
+        <v>10.14854038270859</v>
       </c>
       <c r="G45" t="n">
-        <v>2.22029629114027</v>
+        <v>2.30645602978973</v>
       </c>
       <c r="H45" t="n">
-        <v>6.375478470430767</v>
+        <v>6.403334235929634</v>
       </c>
       <c r="I45" t="n">
-        <v>13.08772342178777</v>
+        <v>13.48400834060052</v>
       </c>
       <c r="J45" t="n">
-        <v>77.44033196026416</v>
+        <v>110.6952820021127</v>
       </c>
       <c r="K45" t="n">
-        <v>-0.1190826705696756</v>
+        <v>-0.1569863158120406</v>
       </c>
       <c r="L45" t="n">
-        <v>29.35887196381957</v>
+        <v>29.53304441179725</v>
       </c>
       <c r="M45" t="n">
-        <v>1.840414374816492</v>
+        <v>1.908465294797607</v>
       </c>
       <c r="N45" t="n">
-        <v>4.578102206070735</v>
+        <v>5.351255889612446</v>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="n">
@@ -2673,38 +2837,42 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9.35625643537924</v>
+        <v>9.388159488048043</v>
       </c>
       <c r="D46" t="n">
-        <v>6.519786466641172</v>
-      </c>
-      <c r="E46" t="inlineStr"/>
+        <v>6.365234746060896</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F46" t="n">
-        <v>10.02982898849187</v>
+        <v>10.04028226270403</v>
       </c>
       <c r="G46" t="n">
-        <v>2.313733175115669</v>
+        <v>2.303539763785875</v>
       </c>
       <c r="H46" t="n">
-        <v>6.519786466641172</v>
+        <v>6.365234746060896</v>
       </c>
       <c r="I46" t="n">
-        <v>13.30850893781226</v>
+        <v>13.48994560320303</v>
       </c>
       <c r="J46" t="n">
-        <v>90.76633641608677</v>
+        <v>92</v>
       </c>
       <c r="K46" t="n">
-        <v>-0.3648938324790788</v>
+        <v>-0.02636678376514239</v>
       </c>
       <c r="L46" t="n">
-        <v>29.05439571075168</v>
+        <v>29.46673518542422</v>
       </c>
       <c r="M46" t="n">
-        <v>1.910454526161541</v>
+        <v>1.918165482131047</v>
       </c>
       <c r="N46" t="n">
-        <v>5.351652975842292</v>
+        <v>5.561402060692378</v>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="n">
@@ -2723,38 +2891,42 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4.305676637170441</v>
+        <v>4.30546698802885</v>
       </c>
       <c r="D47" t="n">
-        <v>4.218243260829583</v>
-      </c>
-      <c r="E47" t="inlineStr"/>
+        <v>4.229469824081604</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F47" t="n">
-        <v>1.798251351274791</v>
+        <v>1.835127727847425</v>
       </c>
       <c r="G47" t="n">
-        <v>3.044662908393708</v>
+        <v>3.033912822618919</v>
       </c>
       <c r="H47" t="n">
-        <v>4.218243260829583</v>
+        <v>4.229469824081604</v>
       </c>
       <c r="I47" t="n">
-        <v>5.488036435820352</v>
+        <v>5.503669742048901</v>
       </c>
       <c r="J47" t="n">
-        <v>11.98009132838729</v>
+        <v>11.93751761474438</v>
       </c>
       <c r="K47" t="n">
-        <v>1.485624348458162</v>
+        <v>1.38873965881396</v>
       </c>
       <c r="L47" t="n">
-        <v>7.326293017774177</v>
+        <v>7.428819327246064</v>
       </c>
       <c r="M47" t="n">
-        <v>0.2255371228001486</v>
+        <v>0.2152070306586568</v>
       </c>
       <c r="N47" t="n">
-        <v>0.1057887676740354</v>
+        <v>0.07232227844628936</v>
       </c>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="n">
@@ -2773,38 +2945,42 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4.34126623157907</v>
+        <v>4.300295350319518</v>
       </c>
       <c r="D48" t="n">
-        <v>4.261500764465588</v>
-      </c>
-      <c r="E48" t="inlineStr"/>
+        <v>4.239543460952484</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F48" t="n">
-        <v>1.800763134986625</v>
+        <v>1.832631665649957</v>
       </c>
       <c r="G48" t="n">
-        <v>3.126891165503854</v>
+        <v>3.034002326813767</v>
       </c>
       <c r="H48" t="n">
-        <v>4.261500764465588</v>
+        <v>4.239543460952484</v>
       </c>
       <c r="I48" t="n">
-        <v>5.491876546533117</v>
+        <v>5.502525097834901</v>
       </c>
       <c r="J48" t="n">
-        <v>12.49106773436139</v>
+        <v>13.37003686904954</v>
       </c>
       <c r="K48" t="n">
-        <v>1.4841087685282</v>
+        <v>1.380735839689131</v>
       </c>
       <c r="L48" t="n">
-        <v>7.4340248545048</v>
+        <v>7.398083726216695</v>
       </c>
       <c r="M48" t="n">
-        <v>0.2629198407315386</v>
+        <v>0.2033801892366767</v>
       </c>
       <c r="N48" t="n">
-        <v>0.1371019063074428</v>
+        <v>0.09292835449953696</v>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="n">
@@ -2823,38 +2999,42 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4.315585198292449</v>
+        <v>4.307613079015273</v>
       </c>
       <c r="D49" t="n">
-        <v>4.266035470446788</v>
-      </c>
-      <c r="E49" t="inlineStr"/>
+        <v>4.236459535859181</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F49" t="n">
-        <v>1.853164373124682</v>
+        <v>1.839405664565108</v>
       </c>
       <c r="G49" t="n">
-        <v>3.037524462995006</v>
+        <v>3.039299387217432</v>
       </c>
       <c r="H49" t="n">
-        <v>4.266035470446788</v>
+        <v>4.236459535859181</v>
       </c>
       <c r="I49" t="n">
-        <v>5.537917925082236</v>
+        <v>5.504837447432477</v>
       </c>
       <c r="J49" t="n">
-        <v>11.74445891409608</v>
+        <v>12.77981096876993</v>
       </c>
       <c r="K49" t="n">
-        <v>1.370949354819505</v>
+        <v>1.376423975675771</v>
       </c>
       <c r="L49" t="n">
-        <v>7.468436441735403</v>
+        <v>7.441541049323803</v>
       </c>
       <c r="M49" t="n">
-        <v>0.1874102004428653</v>
+        <v>0.22479667007431</v>
       </c>
       <c r="N49" t="n">
-        <v>0.09951626844669104</v>
+        <v>0.04989928331146887</v>
       </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="n">
@@ -2873,38 +3053,42 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.325120008601699</v>
+        <v>4.309153769941592</v>
       </c>
       <c r="D50" t="n">
-        <v>4.247428434345176</v>
-      </c>
-      <c r="E50" t="inlineStr"/>
+        <v>4.242086685115272</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F50" t="n">
-        <v>1.840758444026</v>
+        <v>1.85537297664003</v>
       </c>
       <c r="G50" t="n">
-        <v>3.030385794840273</v>
+        <v>3.015822476787481</v>
       </c>
       <c r="H50" t="n">
-        <v>4.247428434345176</v>
+        <v>4.242086685115272</v>
       </c>
       <c r="I50" t="n">
-        <v>5.549560342500204</v>
+        <v>5.510835647190048</v>
       </c>
       <c r="J50" t="n">
-        <v>13.34879579567525</v>
+        <v>12.45671535314922</v>
       </c>
       <c r="K50" t="n">
-        <v>1.415633582993924</v>
+        <v>1.38967043531677</v>
       </c>
       <c r="L50" t="n">
-        <v>7.474573703349764</v>
+        <v>7.488316499371546</v>
       </c>
       <c r="M50" t="n">
-        <v>0.2035473457313505</v>
+        <v>0.2389349418229177</v>
       </c>
       <c r="N50" t="n">
-        <v>0.1011170829880732</v>
+        <v>0.08416326887758618</v>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="n">
@@ -2923,38 +3107,42 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.315063260425835</v>
+        <v>4.310204005926959</v>
       </c>
       <c r="D51" t="n">
-        <v>4.241795228427004</v>
-      </c>
-      <c r="E51" t="inlineStr"/>
+        <v>4.239682345799063</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F51" t="n">
-        <v>1.848153270512891</v>
+        <v>1.828268334741789</v>
       </c>
       <c r="G51" t="n">
-        <v>3.024673590535666</v>
+        <v>3.025884045473297</v>
       </c>
       <c r="H51" t="n">
-        <v>4.241795228427004</v>
+        <v>4.239682345799063</v>
       </c>
       <c r="I51" t="n">
-        <v>5.518257505187775</v>
+        <v>5.516967878991715</v>
       </c>
       <c r="J51" t="n">
-        <v>11.6408783727226</v>
+        <v>12.9154010641437</v>
       </c>
       <c r="K51" t="n">
-        <v>1.422404731661222</v>
+        <v>1.41548283731835</v>
       </c>
       <c r="L51" t="n">
-        <v>7.485670592111927</v>
+        <v>7.412739703226372</v>
       </c>
       <c r="M51" t="n">
-        <v>0.207501865301513</v>
+        <v>0.2227590783647983</v>
       </c>
       <c r="N51" t="n">
-        <v>0.09244425541892198</v>
+        <v>0.04370845602805362</v>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="n">
@@ -2973,38 +3161,42 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4.307620638192007</v>
+        <v>4.298367005391075</v>
       </c>
       <c r="D52" t="n">
-        <v>4.221638902171811</v>
-      </c>
-      <c r="E52" t="inlineStr"/>
+        <v>4.225716838640047</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F52" t="n">
-        <v>1.810513863465639</v>
+        <v>1.842890389016198</v>
       </c>
       <c r="G52" t="n">
-        <v>3.058095443208972</v>
+        <v>3.01531331433435</v>
       </c>
       <c r="H52" t="n">
-        <v>4.221638902171811</v>
+        <v>4.225716838640047</v>
       </c>
       <c r="I52" t="n">
-        <v>5.463286283602745</v>
+        <v>5.498123300697851</v>
       </c>
       <c r="J52" t="n">
-        <v>11.86652404743627</v>
+        <v>13.00326553115182</v>
       </c>
       <c r="K52" t="n">
-        <v>1.475730459260055</v>
+        <v>1.380216322909567</v>
       </c>
       <c r="L52" t="n">
-        <v>7.415982675128988</v>
+        <v>7.456871991495508</v>
       </c>
       <c r="M52" t="n">
-        <v>0.3017908924646454</v>
+        <v>0.2194999375321961</v>
       </c>
       <c r="N52" t="n">
-        <v>0.1789392804284184</v>
+        <v>0.0602314195435727</v>
       </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="n">
@@ -3023,38 +3215,42 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4.31769729824091</v>
+        <v>4.299844012520868</v>
       </c>
       <c r="D53" t="n">
-        <v>4.26188738366408</v>
-      </c>
-      <c r="E53" t="inlineStr"/>
+        <v>4.226863299098251</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F53" t="n">
-        <v>1.85448095405193</v>
+        <v>1.83756809667831</v>
       </c>
       <c r="G53" t="n">
-        <v>3.008684706903185</v>
+        <v>3.041427281515171</v>
       </c>
       <c r="H53" t="n">
-        <v>4.26188738366408</v>
+        <v>4.226863299098251</v>
       </c>
       <c r="I53" t="n">
-        <v>5.542970325386394</v>
+        <v>5.487977066558894</v>
       </c>
       <c r="J53" t="n">
-        <v>12.23668366463359</v>
+        <v>14.42401195791946</v>
       </c>
       <c r="K53" t="n">
-        <v>1.389986288128044</v>
+        <v>1.411263943521724</v>
       </c>
       <c r="L53" t="n">
-        <v>7.429413844187841</v>
+        <v>7.466082813437852</v>
       </c>
       <c r="M53" t="n">
-        <v>0.2234840703152837</v>
+        <v>0.2453547176400541</v>
       </c>
       <c r="N53" t="n">
-        <v>0.02131402524211534</v>
+        <v>0.1416383435578066</v>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="n">
@@ -3073,38 +3269,42 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4.286463470387129</v>
+        <v>4.310760315020895</v>
       </c>
       <c r="D54" t="n">
-        <v>4.203333384299891</v>
-      </c>
-      <c r="E54" t="inlineStr"/>
+        <v>4.232558796537095</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F54" t="n">
-        <v>1.846199487172267</v>
+        <v>1.854333937988177</v>
       </c>
       <c r="G54" t="n">
-        <v>3.016540533139552</v>
+        <v>3.021247359275719</v>
       </c>
       <c r="H54" t="n">
-        <v>4.203333384299891</v>
+        <v>4.232558796537095</v>
       </c>
       <c r="I54" t="n">
-        <v>5.414922441162204</v>
+        <v>5.51160170493352</v>
       </c>
       <c r="J54" t="n">
-        <v>11.92116886477008</v>
+        <v>13.09290363797568</v>
       </c>
       <c r="K54" t="n">
-        <v>1.447375692839431</v>
+        <v>1.397317292777807</v>
       </c>
       <c r="L54" t="n">
-        <v>7.530286533663862</v>
+        <v>7.451407943539638</v>
       </c>
       <c r="M54" t="n">
-        <v>0.3044085339532651</v>
+        <v>0.2557994226801252</v>
       </c>
       <c r="N54" t="n">
-        <v>0.2641358824599407</v>
+        <v>0.0969983996103756</v>
       </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="n">
@@ -3123,38 +3323,42 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>4.321305794224852</v>
+        <v>4.310878108637112</v>
       </c>
       <c r="D55" t="n">
-        <v>4.274961893273298</v>
-      </c>
-      <c r="E55" t="inlineStr"/>
+        <v>4.231023552349669</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F55" t="n">
-        <v>1.82209474039309</v>
+        <v>1.832234329698845</v>
       </c>
       <c r="G55" t="n">
-        <v>3.04829559697224</v>
+        <v>3.055961206254199</v>
       </c>
       <c r="H55" t="n">
-        <v>4.274961893273298</v>
+        <v>4.231023552349669</v>
       </c>
       <c r="I55" t="n">
-        <v>5.504342892888566</v>
+        <v>5.503946491772272</v>
       </c>
       <c r="J55" t="n">
-        <v>11.87391584050962</v>
+        <v>12.7417903833533</v>
       </c>
       <c r="K55" t="n">
-        <v>1.397940830348525</v>
+        <v>1.372778595441719</v>
       </c>
       <c r="L55" t="n">
-        <v>7.395990656715668</v>
+        <v>7.450078437500428</v>
       </c>
       <c r="M55" t="n">
-        <v>0.176647036121027</v>
+        <v>0.224912580109831</v>
       </c>
       <c r="N55" t="n">
-        <v>0.01378271025704292</v>
+        <v>0.05668999347403103</v>
       </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="n">
@@ -3173,38 +3377,42 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>4.310122192209233</v>
+        <v>4.318548682545922</v>
       </c>
       <c r="D56" t="n">
-        <v>4.225049248500507</v>
-      </c>
-      <c r="E56" t="inlineStr"/>
+        <v>4.259373566231206</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F56" t="n">
-        <v>1.865617026805063</v>
+        <v>1.840504920856205</v>
       </c>
       <c r="G56" t="n">
-        <v>3.017062235337129</v>
+        <v>3.042160865410439</v>
       </c>
       <c r="H56" t="n">
-        <v>4.225049248500507</v>
+        <v>4.259373566231206</v>
       </c>
       <c r="I56" t="n">
-        <v>5.501183958389444</v>
+        <v>5.535112474159563</v>
       </c>
       <c r="J56" t="n">
-        <v>13.45715623100013</v>
+        <v>13.08282732997528</v>
       </c>
       <c r="K56" t="n">
-        <v>1.416469949092225</v>
+        <v>1.421977924009542</v>
       </c>
       <c r="L56" t="n">
-        <v>7.507907695474124</v>
+        <v>7.439105312392616</v>
       </c>
       <c r="M56" t="n">
-        <v>0.2860424874385897</v>
+        <v>0.2453057396199266</v>
       </c>
       <c r="N56" t="n">
-        <v>0.1658160772179351</v>
+        <v>0.1189334822420403</v>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="n">
@@ -3223,38 +3431,42 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>-0.003668926706615035</v>
+        <v>0.005792514738448344</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.01435136660933351</v>
-      </c>
-      <c r="E57" t="inlineStr"/>
+        <v>0.01382906899266741</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No mode</t>
+        </is>
+      </c>
       <c r="F57" t="n">
-        <v>1.000079228860563</v>
+        <v>1.004204522318259</v>
       </c>
       <c r="G57" t="n">
-        <v>-0.6829680403852734</v>
+        <v>-0.6732046050067324</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.01435136660933351</v>
+        <v>0.01382906899266741</v>
       </c>
       <c r="I57" t="n">
-        <v>0.6724509955748268</v>
+        <v>0.6868550713036358</v>
       </c>
       <c r="J57" t="n">
-        <v>3.293128826583638</v>
+        <v>4.2631122352108</v>
       </c>
       <c r="K57" t="n">
-        <v>-1.650628822769477</v>
+        <v>-1.663990183294592</v>
       </c>
       <c r="L57" t="n">
-        <v>1.679572465504314</v>
+        <v>1.641607271564288</v>
       </c>
       <c r="M57" t="n">
-        <v>0.03065552207728061</v>
+        <v>-0.00668711370487553</v>
       </c>
       <c r="N57" t="n">
-        <v>0.008831715875439183</v>
+        <v>-0.03215253033462417</v>
       </c>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="n">
@@ -3310,7 +3522,7 @@
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
-          <t>UPI</t>
+          <t>Debit Card</t>
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
@@ -3344,7 +3556,7 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
@@ -3378,7 +3590,7 @@
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
         <is>
-          <t>No Membership</t>
+          <t>Membership</t>
         </is>
       </c>
       <c r="F61" t="inlineStr"/>

</xml_diff>